<commit_message>
pasay in thousands fixed
</commit_message>
<xml_diff>
--- a/SCBA/2016/NCR/2016_NCR.xlsx
+++ b/SCBA/2016/NCR/2016_NCR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ThesisProject\thesis\SCBA\2016\NCR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Thesis\thesis\SCBA\2016\NCR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6347729C-307F-4DF9-88EF-792487A99ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611E7D67-0365-4AF7-AE98-7A33B6CE3105}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="927" activeTab="10" xr2:uid="{360BF9DE-B15B-43CE-9291-7E05B391F461}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="927" activeTab="4" xr2:uid="{360BF9DE-B15B-43CE-9291-7E05B391F461}"/>
   </bookViews>
   <sheets>
     <sheet name="Taguig" sheetId="13" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="Valenzuela" sheetId="1" r:id="rId15"/>
     <sheet name="Caloocan" sheetId="22" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -293,11 +293,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -566,14 +566,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -583,7 +583,7 @@
     <xf numFmtId="40" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -598,31 +598,31 @@
     <xf numFmtId="40" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -698,56 +698,56 @@
     <xf numFmtId="4" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="18" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="41" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="3" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="25" fillId="0" borderId="3" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1088,7 +1088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E6C5C4-4851-4501-8CBC-46F97AF0BA09}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F94" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -3548,7 +3548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE3B46A-E9B9-48A2-B2C7-7C8FF621DB3E}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:I3"/>
     </sheetView>
   </sheetViews>
@@ -11924,7 +11924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860B7B00-B176-4975-B8B3-03ACAA44EF03}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G97" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -14312,8 +14312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09E654E-E438-4860-9BB8-3BA839520E51}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G96" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14438,7 +14438,7 @@
         <v>23</v>
       </c>
       <c r="E11" s="48">
-        <v>964653</v>
+        <v>964653000</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -14449,7 +14449,7 @@
         <v>24</v>
       </c>
       <c r="E12" s="48">
-        <v>1444711</v>
+        <v>1444711000</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -14460,7 +14460,7 @@
         <v>25</v>
       </c>
       <c r="E13" s="49">
-        <v>43033</v>
+        <v>43033000</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -14472,7 +14472,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="19">
         <f t="shared" ref="E14" si="0">SUM(E11:E13)</f>
-        <v>2452397</v>
+        <v>2452397000</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -14492,7 +14492,7 @@
         <v>26</v>
       </c>
       <c r="E16" s="48">
-        <v>159460</v>
+        <v>159460000</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14503,7 +14503,7 @@
         <v>27</v>
       </c>
       <c r="E17" s="48">
-        <v>182616</v>
+        <v>182616000</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14514,7 +14514,7 @@
         <v>28</v>
       </c>
       <c r="E18" s="48">
-        <v>1346</v>
+        <v>1346000</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14526,7 +14526,7 @@
       <c r="D19" s="8"/>
       <c r="E19" s="19">
         <f t="shared" ref="E19" si="1">SUM(E16:E18)</f>
-        <v>343422</v>
+        <v>343422000</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14546,7 +14546,7 @@
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="48">
-        <v>692291</v>
+        <v>692291000</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14579,7 +14579,7 @@
         <v>33</v>
       </c>
       <c r="E24" s="49">
-        <v>61211</v>
+        <v>61211000</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14632,7 +14632,7 @@
         <v>38</v>
       </c>
       <c r="E29" s="49">
-        <v>56100</v>
+        <v>56100000</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14643,7 +14643,7 @@
         <v>39</v>
       </c>
       <c r="E30" s="49">
-        <v>143</v>
+        <v>143000</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14674,7 +14674,7 @@
         <v>42</v>
       </c>
       <c r="E33" s="49">
-        <v>18</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14685,7 +14685,7 @@
         <v>43</v>
       </c>
       <c r="E34" s="50">
-        <v>15002</v>
+        <v>15002000</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14707,7 +14707,7 @@
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="50">
-        <v>373363.77070999995</v>
+        <v>3733630003.77071</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14719,7 +14719,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="19">
         <f>SUM(E14,E19,E21:E36)</f>
-        <v>3993947.7707099998</v>
+        <v>7354214003.77071</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14764,7 +14764,7 @@
         <v>10</v>
       </c>
       <c r="E42" s="51">
-        <v>506629.56456999999</v>
+        <v>506629000.56457001</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14775,7 +14775,7 @@
         <v>11</v>
       </c>
       <c r="E43" s="51">
-        <v>566204.10733999999</v>
+        <v>566204000.10733998</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14786,7 +14786,7 @@
         <v>12</v>
       </c>
       <c r="E44" s="51">
-        <v>14488.88725</v>
+        <v>14488000.887250001</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14806,7 +14806,7 @@
         <v>10</v>
       </c>
       <c r="E46" s="51">
-        <v>49776.392469999999</v>
+        <v>49776000.392470002</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14817,7 +14817,7 @@
         <v>11</v>
       </c>
       <c r="E47" s="51">
-        <v>104416.0186</v>
+        <v>104416000.0186</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14848,7 +14848,7 @@
         <v>10</v>
       </c>
       <c r="E50" s="48">
-        <v>276128.11499000003</v>
+        <v>276128000.11499</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14859,7 +14859,7 @@
         <v>11</v>
       </c>
       <c r="E51" s="48">
-        <v>417285.53100000002</v>
+        <v>417285000.53100002</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14870,7 +14870,7 @@
         <v>12</v>
       </c>
       <c r="E52" s="48">
-        <v>42983.333319999998</v>
+        <v>42983000.333319999</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14890,7 +14890,7 @@
         <v>10</v>
       </c>
       <c r="E54" s="48">
-        <v>2730.63231</v>
+        <v>2730000.6323099998</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14901,7 +14901,7 @@
         <v>11</v>
       </c>
       <c r="E55" s="48">
-        <v>3923.1801399999999</v>
+        <v>3923000.1801399998</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14932,7 +14932,7 @@
         <v>10</v>
       </c>
       <c r="E58" s="52">
-        <v>32773.810120000002</v>
+        <v>32773000.810120001</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14943,7 +14943,7 @@
         <v>11</v>
       </c>
       <c r="E59" s="48">
-        <v>424506.45673999999</v>
+        <v>424506000.45674002</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14954,7 +14954,7 @@
         <v>12</v>
       </c>
       <c r="E60" s="48">
-        <v>28419.405360000001</v>
+        <v>28419000.405359998</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14974,7 +14974,7 @@
         <v>10</v>
       </c>
       <c r="E62" s="48">
-        <v>66348.35070000001</v>
+        <v>66348000.350699998</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14985,7 +14985,7 @@
         <v>11</v>
       </c>
       <c r="E63" s="48">
-        <v>40321.825090000006</v>
+        <v>40321000.825089999</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -14996,7 +14996,7 @@
         <v>12</v>
       </c>
       <c r="E64" s="48">
-        <v>1171.1990000000001</v>
+        <v>1171000.199</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -15015,7 +15015,7 @@
         <v>10</v>
       </c>
       <c r="E66" s="48">
-        <v>135656.30765</v>
+        <v>135656000.30765</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -15026,7 +15026,7 @@
         <v>11</v>
       </c>
       <c r="E67" s="48">
-        <v>128036.67774</v>
+        <v>128036000.67773999</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -15064,7 +15064,7 @@
         <v>11</v>
       </c>
       <c r="E71" s="48">
-        <v>130776.77073</v>
+        <v>130776000.77073</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -15102,7 +15102,7 @@
         <v>47</v>
       </c>
       <c r="E75" s="48">
-        <v>148760.42347000001</v>
+        <v>148760000.42346999</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -15113,7 +15113,7 @@
         <v>48</v>
       </c>
       <c r="E76" s="48">
-        <v>48255.19844</v>
+        <v>48255000.19844</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -15133,7 +15133,7 @@
         <v>49</v>
       </c>
       <c r="E78" s="48">
-        <v>576.25</v>
+        <v>576000.25</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -15171,7 +15171,7 @@
         <v>50</v>
       </c>
       <c r="E82" s="48">
-        <v>60010.513679999996</v>
+        <v>60010000.513680004</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -15285,7 +15285,7 @@
       <c r="D93" s="8"/>
       <c r="E93" s="30">
         <f>SUM(E41:E92)</f>
-        <v>3230178.95071</v>
+        <v>3230169009.9507103</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -15316,7 +15316,7 @@
         <v>12</v>
       </c>
       <c r="E96" s="51">
-        <v>32549.808000000001</v>
+        <v>32549000.807999998</v>
       </c>
       <c r="F96" s="10"/>
       <c r="G96" s="8"/>
@@ -15360,7 +15360,7 @@
         <v>12</v>
       </c>
       <c r="E100" s="51">
-        <v>56326.498390000001</v>
+        <v>56326000.498389997</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15396,7 +15396,7 @@
         <v>12</v>
       </c>
       <c r="E104" s="51">
-        <v>339524.61612000002</v>
+        <v>339524000.61611998</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -15414,7 +15414,7 @@
         <v>12</v>
       </c>
       <c r="E106" s="51">
-        <v>28219.59792</v>
+        <v>28219000.597920001</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -15432,7 +15432,7 @@
         <v>12</v>
       </c>
       <c r="E108" s="51">
-        <v>2123.4149300000004</v>
+        <v>2123000.41493</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -15451,7 +15451,7 @@
         <v>12</v>
       </c>
       <c r="E110" s="45">
-        <v>34302</v>
+        <v>34302000</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -15460,7 +15460,7 @@
       </c>
       <c r="E111" s="44">
         <f>SUM(E95:E110)</f>
-        <v>493045.93536000006</v>
+        <v>493043002.93535995</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -15472,7 +15472,7 @@
       <c r="D112" s="17"/>
       <c r="E112" s="31">
         <f>SUM(E93,E111)</f>
-        <v>3723224.88607</v>
+        <v>3723212012.8860703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>